<commit_message>
Added IF / ELSEIF / ELSE control block
There are some slippery parts about python output, but it is functional.
Java output has not been updated for many commits. Assume not working.
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="108">
   <si>
     <t>→</t>
   </si>
@@ -333,6 +333,21 @@
   </si>
   <si>
     <t>_OP_ _EXPR_ | epsilon</t>
+  </si>
+  <si>
+    <t>elseif</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>"if"</t>
+  </si>
+  <si>
+    <t>"elseif"</t>
+  </si>
+  <si>
+    <t>"else"</t>
   </si>
 </sst>
 </file>
@@ -675,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,12 +701,12 @@
     <col min="1" max="1" width="14.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="77.44140625" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" customWidth="1"/>
-    <col min="7" max="7" width="35.109375" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
@@ -705,7 +720,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>75</v>
       </c>
@@ -722,8 +737,9 @@
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>76</v>
       </c>
@@ -740,8 +756,9 @@
       <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>77</v>
       </c>
@@ -758,8 +775,9 @@
       <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
@@ -776,8 +794,9 @@
       <c r="F5" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>79</v>
       </c>
@@ -794,8 +813,9 @@
       <c r="F6" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>80</v>
       </c>
@@ -812,8 +832,9 @@
       <c r="F7" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>81</v>
       </c>
@@ -830,8 +851,9 @@
       <c r="F8" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>82</v>
       </c>
@@ -848,8 +870,9 @@
       <c r="F9" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>83</v>
       </c>
@@ -866,8 +889,9 @@
       <c r="F10" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>84</v>
       </c>
@@ -885,7 +909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>85</v>
       </c>
@@ -903,7 +927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>86</v>
       </c>
@@ -921,7 +945,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>87</v>
       </c>
@@ -939,7 +963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>88</v>
       </c>
@@ -957,7 +981,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>89</v>
       </c>
@@ -975,13 +999,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>1</v>
       </c>
@@ -989,7 +1010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
@@ -1000,7 +1021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -1011,7 +1032,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>20</v>
       </c>
@@ -1022,7 +1043,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1033,7 +1054,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>36</v>
       </c>
@@ -1044,7 +1065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>38</v>
       </c>
@@ -1055,7 +1076,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>40</v>
       </c>
@@ -1066,7 +1087,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>6</v>
       </c>
@@ -1077,7 +1098,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>43</v>
       </c>
@@ -1088,7 +1109,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>45</v>
       </c>
@@ -1099,7 +1120,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>47</v>
       </c>
@@ -1244,12 +1265,45 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="3" t="s">
+      <c r="B48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Prepared everything for adding functions
And created a drawio file to represent the CFG. It's pretty cool. You
should check it out. Furthermore, see the SECOND TAB of CFG.xlsx for
info on CFG w/ functions.
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14988" windowHeight="9120"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14988" windowHeight="9120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="WithFunctions" sheetId="3" r:id="rId2"/>
+    <sheet name="Backup" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="165">
   <si>
     <t>→</t>
   </si>
@@ -348,13 +350,184 @@
   </si>
   <si>
     <t>"else"</t>
+  </si>
+  <si>
+    <t>_FUNCDEF_</t>
+  </si>
+  <si>
+    <t>_BLOCKSTMT_</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>commonFollow2</t>
+  </si>
+  <si>
+    <t>commonFollow1</t>
+  </si>
+  <si>
+    <t>_FUNCDEF_ _STMTS_ | _IF_ _STMTS_ | _BLOCKSTMT_ _STMTS_ | epsilon</t>
+  </si>
+  <si>
+    <t>_PARAMS0_</t>
+  </si>
+  <si>
+    <t>_PARAMS1_</t>
+  </si>
+  <si>
+    <t>function var (_PARAMS0_) _BLOCKSTMT_</t>
+  </si>
+  <si>
+    <t>_VALUE_</t>
+  </si>
+  <si>
+    <t>(_EXPR_) | _VALUE_ _OPEXPR_</t>
+  </si>
+  <si>
+    <t>_BLOCKSTMT_ _ELSEIF_</t>
+  </si>
+  <si>
+    <t>_FUNCCALL_</t>
+  </si>
+  <si>
+    <t>_ARGS0_</t>
+  </si>
+  <si>
+    <t>_ARGS1_</t>
+  </si>
+  <si>
+    <t>comma</t>
+  </si>
+  <si>
+    <t>","</t>
+  </si>
+  <si>
+    <t>_VALUE_ _ARGS1_ | epsilon</t>
+  </si>
+  <si>
+    <t>, _VALUE_ _ARGS1_ | epsilon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = _EXPR_</t>
+  </si>
+  <si>
+    <t>( _ARGS0_ )</t>
+  </si>
+  <si>
+    <t>_VAR_</t>
+  </si>
+  <si>
+    <t>_FUNCCALL_ | epsilon</t>
+  </si>
+  <si>
+    <t>_VAR_ | _LITERAL_</t>
+  </si>
+  <si>
+    <t>(, epsilon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =, (</t>
+  </si>
+  <si>
+    <t>var _PARAMS1_ | epsilon</t>
+  </si>
+  <si>
+    <t>comma, epsilon</t>
+  </si>
+  <si>
+    <t>, var _PARAMS1_ | epsilon</t>
+  </si>
+  <si>
+    <t>var, epsilon</t>
+  </si>
+  <si>
+    <t>_VARSTMT_</t>
+  </si>
+  <si>
+    <t>_ECHO_; | var _VARSTMT_;</t>
+  </si>
+  <si>
+    <t>var _VAREXPR_</t>
+  </si>
+  <si>
+    <t>_VAREXPR_</t>
+  </si>
+  <si>
+    <t>elseif ( _EXPR_ )  _THEN_ | else _BLOCKSTMT_ | epsilon</t>
+  </si>
+  <si>
+    <t>_VARDEF_ | _FUNCCALL_</t>
+  </si>
+  <si>
+    <t>_VARDEF_</t>
+  </si>
+  <si>
+    <t>"=" (indicates variable definition)</t>
+  </si>
+  <si>
+    <t>vardef</t>
+  </si>
+  <si>
+    <t>&lt;primitives&gt;</t>
+  </si>
+  <si>
+    <t>var, &lt;primitives&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ops&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ops&gt;, epsilon</t>
+  </si>
+  <si>
+    <t>(, var, &lt;primitives&gt;</t>
+  </si>
+  <si>
+    <t>var, &lt;primitives&gt;, epsilon</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =</t>
+  </si>
+  <si>
+    <t>"function"</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>&lt;stmts&gt;</t>
+  </si>
+  <si>
+    <t>{, &lt;stmts&gt;</t>
+  </si>
+  <si>
+    <t>function, if, {, &lt;stmts&gt;, epsilon</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>&lt;ops&gt;, comma, ), ;</t>
+  </si>
+  <si>
+    <t>EOF, _STMTS_.first</t>
+  </si>
+  <si>
+    <t>EOF, _STMTS_.first, elseif, else</t>
+  </si>
+  <si>
+    <t>), ;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,13 +543,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -391,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -410,6 +623,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1311,4 +1557,1495 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="77.44140625" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="6" max="6" width="39.6640625" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F26" s="16" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="20"/>
+      <c r="E32" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="20"/>
+      <c r="E40" s="21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="20"/>
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="21"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="20"/>
+      <c r="E48" s="21"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="21"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="20"/>
+      <c r="E51" s="21"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="D52" s="20"/>
+      <c r="E52" s="21"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D53" s="20"/>
+      <c r="E53" s="21"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="21"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="E45:E54"/>
+    <mergeCell ref="E40:E41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="77.44140625" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="6" max="6" width="27.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Functions added to CFG
Additionally, many verbose options have been updated.
Finally, some memory-saving modifications were made in ParseNode
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="165">
   <si>
     <t>→</t>
   </si>
@@ -466,9 +466,6 @@
     <t>"=" (indicates variable definition)</t>
   </si>
   <si>
-    <t>vardef</t>
-  </si>
-  <si>
     <t>&lt;primitives&gt;</t>
   </si>
   <si>
@@ -511,23 +508,26 @@
     <t>*</t>
   </si>
   <si>
-    <t>&lt;ops&gt;, comma, ), ;</t>
-  </si>
-  <si>
     <t>EOF, _STMTS_.first</t>
   </si>
   <si>
     <t>EOF, _STMTS_.first, elseif, else</t>
   </si>
   <si>
-    <t>), ;</t>
+    <t>&lt;ops&gt;, ;, comma, )</t>
+  </si>
+  <si>
+    <t>commonFollow3</t>
+  </si>
+  <si>
+    <t>eqeq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,28 +544,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -610,7 +588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -629,27 +607,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -661,7 +619,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -673,6 +630,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,7 +922,7 @@
   <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1578,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G60"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1608,838 +1574,828 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+    </row>
+    <row r="3" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="22" t="s">
-        <v>159</v>
+      <c r="E3" s="8" t="s">
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="22" t="s">
+      <c r="G19" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="F24" s="8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="G25" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="16" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F26" s="16" t="s">
-        <v>161</v>
-      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A28" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B29" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>32</v>
       </c>
     </row>
+    <row r="31" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>123</v>
+      <c r="A34" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>145</v>
+      <c r="C34" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>48</v>
+      <c r="A37" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="12"/>
+      <c r="E37" s="13" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>70</v>
-      </c>
+      <c r="A38" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>72</v>
-      </c>
+      <c r="A39" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D39" s="12"/>
+      <c r="E39" s="13"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="21" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="D41" s="20"/>
-      <c r="E41" s="21"/>
+      <c r="A40" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="21"/>
+      <c r="A42" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D43" s="20"/>
-      <c r="E43" s="21"/>
+      <c r="A43" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="10" t="s">
-        <v>110</v>
+      <c r="A44" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="8" t="s">
-        <v>155</v>
+      <c r="C44" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>105</v>
+      <c r="A45" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="13" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>106</v>
-      </c>
+      <c r="A46" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>107</v>
+      <c r="A47" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="18"/>
+      <c r="E47" s="14" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="21" t="s">
-        <v>157</v>
-      </c>
+      <c r="A48" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="18"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
+      <c r="A49" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D49" s="18"/>
+      <c r="E49" s="14"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" s="27"/>
-      <c r="E50" s="23" t="s">
-        <v>149</v>
-      </c>
+      <c r="A50" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="18"/>
+      <c r="E50" s="14"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="D51" s="27"/>
-      <c r="E51" s="23"/>
+      <c r="A51" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="18"/>
+      <c r="E51" s="14"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="27"/>
-      <c r="E52" s="23"/>
+      <c r="A52" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D52" s="18"/>
+      <c r="E52" s="14"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="23"/>
+      <c r="A53" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D53" s="18"/>
+      <c r="E53" s="14"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D54" s="27"/>
-      <c r="E54" s="23"/>
+      <c r="A54" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="18"/>
+      <c r="E54" s="14"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="23"/>
+      <c r="A55" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="18"/>
+      <c r="E55" s="14"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="D56" s="27"/>
-      <c r="E56" s="23"/>
+      <c r="A56" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D56" s="18"/>
+      <c r="E56" s="14"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D57" s="27"/>
-      <c r="E57" s="23"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="D58" s="27"/>
-      <c r="E58" s="23"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="D59" s="27"/>
-      <c r="E59" s="23"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
+      <c r="A57" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="19" t="s">
+      <c r="B57" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E40:E43"/>
-    <mergeCell ref="E50:E59"/>
-    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="E37:E40"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="E47:E56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Eclipse acting buggy. Better commit.
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="211">
   <si>
     <t>→</t>
   </si>
@@ -397,9 +397,6 @@
     <t>_ARGS1_</t>
   </si>
   <si>
-    <t>comma</t>
-  </si>
-  <si>
     <t>","</t>
   </si>
   <si>
@@ -517,9 +514,6 @@
     <t>commonFollow3</t>
   </si>
   <si>
-    <t>eqeq</t>
-  </si>
-  <si>
     <t>_ECHO_; | _INPUT_ var | var _VARSTMT_;</t>
   </si>
   <si>
@@ -533,13 +527,145 @@
   </si>
   <si>
     <t>"input"</t>
+  </si>
+  <si>
+    <t>_EXPRRANK0_</t>
+  </si>
+  <si>
+    <t>_EXPRRANK1_</t>
+  </si>
+  <si>
+    <t>_EXPRRANK2_</t>
+  </si>
+  <si>
+    <t>_EXPRRANK0</t>
+  </si>
+  <si>
+    <t>_OPRANK0_</t>
+  </si>
+  <si>
+    <t>_OPRANK1_</t>
+  </si>
+  <si>
+    <t>_OPRANK2_</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + | -</t>
+  </si>
+  <si>
+    <t>* | /</t>
+  </si>
+  <si>
+    <t>!= | &lt;= | &gt;= | &lt; | &gt; | ==</t>
+  </si>
+  <si>
+    <t>_EXPRRANK1_ _OPRANK0_ _EXPRRANK0_</t>
+  </si>
+  <si>
+    <t>_EXPRRANK2_ _OPRANK1_ _EXPRRANK1_</t>
+  </si>
+  <si>
+    <t>_VALUE_ _OPRANK2_ _EXPRRANK2_</t>
+  </si>
+  <si>
+    <t>"["</t>
+  </si>
+  <si>
+    <t>"]"</t>
+  </si>
+  <si>
+    <t>EMPTY</t>
+  </si>
+  <si>
+    <t>SEMILCOLON</t>
+  </si>
+  <si>
+    <t>COMMA</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>PAREN_OPEN</t>
+  </si>
+  <si>
+    <t>PAREN_CLOSE</t>
+  </si>
+  <si>
+    <t>CURLY_OPEN</t>
+  </si>
+  <si>
+    <t>CURLY_CLOSE</t>
+  </si>
+  <si>
+    <t>SQUARE_OPEN</t>
+  </si>
+  <si>
+    <t>SQUARE_CLOSE</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>STRING</t>
+  </si>
+  <si>
+    <t>FUNCTION</t>
+  </si>
+  <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>ELSEIF</t>
+  </si>
+  <si>
+    <t>ELSE</t>
+  </si>
+  <si>
+    <t>ECHO</t>
+  </si>
+  <si>
+    <t>INPUT</t>
+  </si>
+  <si>
+    <t>VAR</t>
+  </si>
+  <si>
+    <t>ASTERISK</t>
+  </si>
+  <si>
+    <t>SLASH</t>
+  </si>
+  <si>
+    <t>PLUS</t>
+  </si>
+  <si>
+    <t>MINUS</t>
+  </si>
+  <si>
+    <t>NEQ</t>
+  </si>
+  <si>
+    <t>LTEQ</t>
+  </si>
+  <si>
+    <t>GTEQ</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>EQEQ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -561,8 +687,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -587,6 +720,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -600,7 +745,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -650,6 +795,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1556,10 +1707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1597,7 +1748,7 @@
         <v>90</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -1614,7 +1765,7 @@
         <v>113</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>17</v>
@@ -1634,7 +1785,7 @@
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>112</v>
@@ -1648,13 +1799,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1665,13 +1816,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1688,7 +1839,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>112</v>
@@ -1705,10 +1856,10 @@
         <v>119</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
@@ -1722,13 +1873,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>112</v>
@@ -1745,10 +1896,10 @@
         <v>97</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>111</v>
@@ -1768,7 +1919,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>111</v>
@@ -1782,13 +1933,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>111</v>
@@ -1813,16 +1964,16 @@
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>167</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>12</v>
@@ -1830,16 +1981,16 @@
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>12</v>
@@ -1847,23 +1998,23 @@
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="22" t="s">
         <v>86</v>
       </c>
       <c r="B17" s="17" t="s">
@@ -1873,17 +2024,17 @@
         <v>118</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="22" t="s">
         <v>87</v>
       </c>
       <c r="B18" s="17" t="s">
@@ -1893,553 +2044,639 @@
         <v>102</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="s">
+      <c r="B23" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="F19" s="8" t="s">
+      <c r="E23" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
+        <v>171</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="8" t="s">
+      <c r="F31" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="G33" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
-        <v>120</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B26" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F27" s="8"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F34" s="8"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="3" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="18" t="s">
+    <row r="39" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8" t="s">
+    </row>
+    <row r="40" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="20" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="20" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="11" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="20"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="20"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="20"/>
-    </row>
-    <row r="42" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="20"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>42</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="20"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="16"/>
-      <c r="E49" s="21" t="s">
-        <v>147</v>
-      </c>
+      <c r="A49" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="20"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D50" s="16"/>
-      <c r="E50" s="21"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D51" s="16"/>
-      <c r="E51" s="21"/>
+      <c r="A50" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="20"/>
+    </row>
+    <row r="51" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="21"/>
+      <c r="A52" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B53" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D53" s="16"/>
-      <c r="E53" s="21"/>
+      <c r="A53" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B54" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="16"/>
-      <c r="E54" s="21"/>
+      <c r="A54" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D55" s="16"/>
-      <c r="E55" s="21"/>
+      <c r="A55" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D55" s="12"/>
+      <c r="E55" s="20" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B56" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="21"/>
+      <c r="A56" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="20"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="16"/>
-      <c r="E57" s="21"/>
+      <c r="A57" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="12"/>
+      <c r="E57" s="20"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="13" t="s">
-        <v>163</v>
+        <v>201</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" s="16"/>
+      <c r="E58" s="21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="16"/>
+      <c r="E59" s="21"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="16"/>
+      <c r="E60" s="21"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="B61" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D61" s="16"/>
+      <c r="E61" s="21"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D62" s="16"/>
+      <c r="E62" s="21"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D63" s="16"/>
+      <c r="E63" s="21"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D64" s="16"/>
+      <c r="E64" s="21"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" s="16"/>
+      <c r="E65" s="21"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D66" s="16"/>
+      <c r="E66" s="21"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D58" s="16"/>
-      <c r="E58" s="21"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="11" t="s">
+      <c r="D67" s="16"/>
+      <c r="E67" s="21"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E38:E41"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="E49:E58"/>
+    <mergeCell ref="E47:E50"/>
+    <mergeCell ref="E55:E57"/>
+    <mergeCell ref="E58:E67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Comments added to language as Terminals
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="209">
   <si>
     <t>→</t>
   </si>
@@ -496,9 +496,6 @@
     <t>commonFollow3</t>
   </si>
   <si>
-    <t>_ECHO_; | _INPUT_ var | var _VARSTMT_;</t>
-  </si>
-  <si>
     <t>_INPUT_</t>
   </si>
   <si>
@@ -647,6 +644,15 @@
   </si>
   <si>
     <t>EOF, }, _STMTS_.first, elseif, else</t>
+  </si>
+  <si>
+    <t>COMMENT</t>
+  </si>
+  <si>
+    <t>_ECHO_; | _INPUT_ var; | var _VARSTMT_; | comment</t>
+  </si>
+  <si>
+    <t>"//" to "\n"</t>
   </si>
 </sst>
 </file>
@@ -793,12 +799,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -806,6 +806,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1713,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1792,7 +1798,7 @@
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>112</v>
@@ -1846,7 +1852,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>112</v>
@@ -1866,7 +1872,7 @@
         <v>152</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
@@ -1886,7 +1892,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>112</v>
@@ -1906,7 +1912,7 @@
         <v>152</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>111</v>
@@ -1926,7 +1932,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>111</v>
@@ -1940,13 +1946,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>151</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>111</v>
@@ -1971,16 +1977,16 @@
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>12</v>
@@ -2028,59 +2034,59 @@
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F18" s="23"/>
+        <v>195</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F19" s="23"/>
+        <v>196</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="F20" s="23"/>
+        <v>197</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>203</v>
+      </c>
+      <c r="F20" s="26"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
@@ -2229,7 +2235,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
@@ -2240,7 +2246,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>0</v>
@@ -2251,7 +2257,7 @@
     </row>
     <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>0</v>
@@ -2262,7 +2268,7 @@
     </row>
     <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>0</v>
@@ -2273,7 +2279,7 @@
     </row>
     <row r="35" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>0</v>
@@ -2284,7 +2290,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
@@ -2295,7 +2301,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>0</v>
@@ -2306,7 +2312,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
@@ -2317,327 +2323,338 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="12"/>
-      <c r="E41" s="24" t="s">
-        <v>143</v>
+      <c r="A41" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="12"/>
+      <c r="E42" s="27" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="24"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="D43" s="12"/>
-      <c r="E43" s="24"/>
+      <c r="E43" s="27"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="12"/>
+      <c r="E44" s="27"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="27"/>
+    </row>
+    <row r="46" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="B44" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="24"/>
-    </row>
-    <row r="45" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="8" t="s">
+      <c r="B46" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="24" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="D50" s="12"/>
-      <c r="E50" s="24"/>
+      <c r="E50" s="27" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="24"/>
+      <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>199</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>145</v>
-      </c>
+      <c r="A52" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B53" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C53" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D53" s="26"/>
-      <c r="E53" s="25"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D54" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="E54" s="25"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="23"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="E55" s="23"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D55" s="27"/>
-      <c r="E55" s="25"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D56" s="26" t="s">
-        <v>201</v>
-      </c>
-      <c r="E56" s="25"/>
+      <c r="D56" s="25"/>
+      <c r="E56" s="23"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D58" s="26"/>
-      <c r="E58" s="25"/>
+        <v>60</v>
+      </c>
+      <c r="D58" s="24"/>
+      <c r="E58" s="23"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="26"/>
-      <c r="E59" s="25"/>
+        <v>62</v>
+      </c>
+      <c r="D59" s="24"/>
+      <c r="E59" s="23"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D60" s="26"/>
-      <c r="E60" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="D60" s="24"/>
+      <c r="E60" s="23"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" s="24"/>
+      <c r="E61" s="23"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D61" s="26"/>
-      <c r="E61" s="25"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="9" t="s">
+      <c r="D62" s="24"/>
+      <c r="E62" s="23"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B62" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="11" t="s">
+      <c r="B63" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D62" s="12"/>
-      <c r="E62" s="12"/>
+      <c r="D63" s="12"/>
+      <c r="E63" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E52:E61"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D61"/>
+    <mergeCell ref="E53:E62"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D57:D62"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E50:E52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated the CFG map and excel spec files as necessary
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -652,7 +652,7 @@
     <t>_ECHO_; | _INPUT_ var; | var _VARSTMT_; | comment</t>
   </si>
   <si>
-    <t>"//" to "\n"</t>
+    <t>"//" to "\r|\n|\f"</t>
   </si>
 </sst>
 </file>
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Expressions may be passed as arguments
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -397,12 +397,6 @@
     <t>","</t>
   </si>
   <si>
-    <t>_VALUE_ _ARGS1_ | epsilon</t>
-  </si>
-  <si>
-    <t>, _VALUE_ _ARGS1_ | epsilon</t>
-  </si>
-  <si>
     <t xml:space="preserve"> = _EXPR_</t>
   </si>
   <si>
@@ -466,9 +460,6 @@
     <t>&lt;ops&gt;</t>
   </si>
   <si>
-    <t>var, &lt;primitives&gt;, epsilon</t>
-  </si>
-  <si>
     <t>(</t>
   </si>
   <si>
@@ -653,6 +644,15 @@
   </si>
   <si>
     <t>"//" to "\r|\n|\f"</t>
+  </si>
+  <si>
+    <t>_EXPR_ _ARGS1_ | epsilon</t>
+  </si>
+  <si>
+    <t>, _EXPR_ _ARGS1_ | epsilon</t>
+  </si>
+  <si>
+    <t>(, var, &lt;primitives&gt;, plus, minus, epsilon</t>
   </si>
 </sst>
 </file>
@@ -1721,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,7 +1761,7 @@
         <v>90</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -1778,7 +1778,7 @@
         <v>113</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>17</v>
@@ -1798,7 +1798,7 @@
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>112</v>
@@ -1812,13 +1812,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1829,13 +1829,13 @@
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1852,7 +1852,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>112</v>
@@ -1869,10 +1869,10 @@
         <v>118</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
@@ -1886,13 +1886,13 @@
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>112</v>
@@ -1909,10 +1909,10 @@
         <v>97</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>111</v>
@@ -1932,7 +1932,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>111</v>
@@ -1946,13 +1946,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>111</v>
@@ -1977,16 +1977,16 @@
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>12</v>
@@ -1994,16 +1994,16 @@
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>12</v>
@@ -2011,16 +2011,16 @@
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>12</v>
@@ -2034,57 +2034,57 @@
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>195</v>
-      </c>
       <c r="E18" s="26" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F18" s="26"/>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>196</v>
-      </c>
       <c r="E19" s="26" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F19" s="26"/>
     </row>
     <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="E20" s="26" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F20" s="26"/>
     </row>
@@ -2096,56 +2096,56 @@
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>130</v>
-      </c>
       <c r="F23" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2156,16 +2156,16 @@
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2176,13 +2176,13 @@
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>123</v>
+        <v>206</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>146</v>
+        <v>208</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2193,13 +2193,13 @@
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2213,13 +2213,13 @@
         <v>8</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2235,7 +2235,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>0</v>
@@ -2246,7 +2246,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>0</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B33" s="13" t="s">
         <v>0</v>
@@ -2268,18 +2268,18 @@
     </row>
     <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B35" s="13" t="s">
         <v>0</v>
@@ -2290,7 +2290,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>0</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>0</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
@@ -2323,35 +2323,35 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="27" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -2384,7 +2384,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>0</v>
@@ -2397,7 +2397,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>0</v>
@@ -2410,18 +2410,18 @@
     </row>
     <row r="46" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B46" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>0</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>0</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>0</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="9" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>0</v>
@@ -2464,38 +2464,38 @@
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="27" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="27"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B52" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B53" s="21" t="s">
         <v>0</v>
@@ -2504,15 +2504,15 @@
         <v>54</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E53" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B54" s="21" t="s">
         <v>0</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>0</v>
@@ -2534,13 +2534,13 @@
         <v>50</v>
       </c>
       <c r="D55" s="25" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="E55" s="23"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B56" s="18" t="s">
         <v>0</v>
@@ -2553,7 +2553,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>0</v>
@@ -2562,13 +2562,13 @@
         <v>58</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E57" s="23"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>0</v>
@@ -2581,7 +2581,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>0</v>
@@ -2594,7 +2594,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>0</v>
@@ -2607,7 +2607,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>0</v>
@@ -2620,7 +2620,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
&& and || added
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="216">
   <si>
     <t>→</t>
   </si>
@@ -595,24 +595,15 @@
     <t>Starts with any a-z, A-Z, or _, following, any combination a-z, A-Z, 0-9, _</t>
   </si>
   <si>
-    <t>__PRECEDENCE0__</t>
-  </si>
-  <si>
     <t>__PRECEDENCE1__</t>
   </si>
   <si>
     <t>__PRECEDENCE2__</t>
   </si>
   <si>
-    <t>__PRECEDENCE0__ &lt;operatorsPrecedence1&gt; __PRECEDENCE1__</t>
-  </si>
-  <si>
     <t>__PRECEDENCE1__ &lt;operatorsPrecedence1&gt; __PRECEDENCE2__</t>
   </si>
   <si>
-    <t>__PRECEDENCE2__ &lt;operatorsPrecedence1&gt; _VALUE_</t>
-  </si>
-  <si>
     <t>Precedence 1</t>
   </si>
   <si>
@@ -653,6 +644,36 @@
   </si>
   <si>
     <t>(, var, &lt;primitives&gt;, plus, minus, epsilon</t>
+  </si>
+  <si>
+    <t>AND</t>
+  </si>
+  <si>
+    <t>"&amp;&amp;"</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>"||"</t>
+  </si>
+  <si>
+    <t>Precedence 4</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE3__</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE3__ &lt;operatorsPrecedence3&gt; __PRECEDENCE4__</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE2__ &lt;operatorsPrecedence2&gt; __PRECEDENCE3__</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE4__</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE4__ &lt;operatorsPrecedence4&gt; _VALUE_</t>
   </si>
 </sst>
 </file>
@@ -745,7 +766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -799,6 +820,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1719,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,7 +1822,7 @@
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>112</v>
@@ -1852,7 +1876,7 @@
         <v>23</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>112</v>
@@ -1872,7 +1896,7 @@
         <v>149</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
@@ -1892,7 +1916,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>112</v>
@@ -1912,7 +1936,7 @@
         <v>149</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>111</v>
@@ -1932,7 +1956,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>111</v>
@@ -1946,13 +1970,13 @@
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>148</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>111</v>
@@ -2037,10 +2061,10 @@
         <v>189</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2051,12 +2075,12 @@
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="F18" s="26"/>
+        <v>191</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
@@ -2066,60 +2090,55 @@
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="F19" s="26"/>
+        <v>213</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F19" s="27"/>
     </row>
     <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="E20" s="26" t="s">
-        <v>200</v>
-      </c>
-      <c r="F20" s="26"/>
+        <v>212</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>117</v>
+      <c r="A21" s="16" t="s">
+        <v>214</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>152</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>6</v>
+        <v>142</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>151</v>
@@ -2130,16 +2149,16 @@
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>151</v>
@@ -2150,16 +2169,16 @@
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>151</v>
@@ -2170,33 +2189,36 @@
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>206</v>
+        <v>124</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>208</v>
+        <v>144</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>147</v>
+        <v>151</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>147</v>
@@ -2204,457 +2226,504 @@
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E28" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F28" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G28" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F28" s="8"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F29" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B33" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8" t="s">
+      <c r="B36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>205</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="27" t="s">
-        <v>141</v>
+      <c r="A42" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="27"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="D44" s="12"/>
-      <c r="E44" s="27"/>
+      <c r="E44" s="28"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D45" s="12"/>
+      <c r="E45" s="28"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="11" t="s">
+      <c r="B46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="27"/>
-    </row>
-    <row r="46" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="14" t="s">
+      <c r="D46" s="12"/>
+      <c r="E46" s="28"/>
+    </row>
+    <row r="47" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B46" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="8" t="s">
+      <c r="B47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B49" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="3" t="s">
+      <c r="B50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="27" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B51" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="D51" s="12"/>
-      <c r="E51" s="27"/>
+      <c r="E51" s="28" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D52" s="12"/>
+      <c r="E52" s="28"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="11" t="s">
+      <c r="B53" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="27"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D53" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="E53" s="23" t="s">
-        <v>143</v>
-      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="28"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="22" t="s">
+      <c r="B55" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D54" s="24"/>
-      <c r="E54" s="23"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D55" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="E55" s="23"/>
+      <c r="D55" s="25"/>
+      <c r="E55" s="24"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="E56" s="24"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B56" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="19" t="s">
+      <c r="B57" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D56" s="25"/>
-      <c r="E56" s="23"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="E57" s="23"/>
+      <c r="D57" s="26"/>
+      <c r="E57" s="24"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B58" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="24"/>
-      <c r="E58" s="23"/>
+        <v>58</v>
+      </c>
+      <c r="D58" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="E58" s="24"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B59" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D59" s="24"/>
-      <c r="E59" s="23"/>
+        <v>60</v>
+      </c>
+      <c r="D59" s="25"/>
+      <c r="E59" s="24"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="D60" s="25"/>
+      <c r="E60" s="24"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D61" s="24"/>
-      <c r="E61" s="23"/>
+        <v>64</v>
+      </c>
+      <c r="D61" s="25"/>
+      <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="25"/>
+      <c r="E62" s="24"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="B62" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="22" t="s">
+      <c r="B63" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D62" s="24"/>
-      <c r="E62" s="23"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
+      <c r="D63" s="25"/>
+      <c r="E63" s="24"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E64" s="23"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="26"/>
+      <c r="E65" s="23"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C63" s="11" t="s">
+      <c r="B66" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D63" s="12"/>
-      <c r="E63" s="12"/>
+      <c r="D66" s="12"/>
+      <c r="E66" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E53:E62"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="D57:D62"/>
+  <mergeCells count="11">
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E54:E63"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D63"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E43:E46"/>
+    <mergeCell ref="E51:E53"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Token.java cleanup and update CFG doc files
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="221">
   <si>
     <t>→</t>
   </si>
@@ -673,7 +673,22 @@
     <t>__PRECEDENCE4__</t>
   </si>
   <si>
-    <t>__PRECEDENCE4__ &lt;operatorsPrecedence4&gt; _VALUE_</t>
+    <t>__PRECEDENCE5__</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE4__ &lt;operatorsPrecedence4&gt; __PRECEDENCE5__</t>
+  </si>
+  <si>
+    <t>_VALUEOREXPR_</t>
+  </si>
+  <si>
+    <t>_VALUE_ | _EXPR_</t>
+  </si>
+  <si>
+    <t>(, var, &lt;primitives&gt;</t>
+  </si>
+  <si>
+    <t>__PRECEDENCE5__ &lt;operatorsPrecedence5&gt; _VALUEOREXPR_</t>
   </si>
 </sst>
 </file>
@@ -1743,10 +1758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2052,45 +2067,50 @@
     </row>
     <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E18" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F18" s="8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F18" s="27"/>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="E19" s="27" t="s">
         <v>197</v>
@@ -2099,13 +2119,13 @@
     </row>
     <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E20" s="27" t="s">
         <v>197</v>
@@ -2114,13 +2134,13 @@
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E21" s="27" t="s">
         <v>197</v>
@@ -2128,57 +2148,45 @@
       <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>117</v>
+      <c r="A22" s="16" t="s">
+        <v>214</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>152</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>0</v>
-      </c>
+      <c r="A23" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B23" s="13"/>
       <c r="C23" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>152</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>197</v>
+      </c>
+      <c r="F23" s="27"/>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="B24" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>151</v>
@@ -2189,16 +2197,16 @@
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>144</v>
+        <v>6</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>151</v>
@@ -2209,521 +2217,562 @@
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>203</v>
+        <v>126</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>205</v>
+        <v>128</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>147</v>
+        <v>151</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>204</v>
+        <v>124</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>147</v>
+        <v>151</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="B30" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F30" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G30" s="8" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F29" s="8"/>
-    </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="F31" s="8"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="3" t="s">
+      <c r="B34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="6" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="B35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B34" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="8" t="s">
+      <c r="B38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="B40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="3" t="s">
+      <c r="B42" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="3" t="s">
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="3" t="s">
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="b">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="B43" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="11" t="s">
+      <c r="B45" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="28" t="s">
+      <c r="D45" s="12"/>
+      <c r="E45" s="28" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="11" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="28"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="28"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="28"/>
     </row>
-    <row r="47" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D47" s="12"/>
+      <c r="E47" s="28"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="12"/>
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
         <v>171</v>
       </c>
-      <c r="B47" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="8" t="s">
+      <c r="B49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="B52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="28"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" s="12"/>
+      <c r="E53" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="12"/>
+      <c r="E54" s="28"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="11" t="s">
+      <c r="B55" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="28"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="20" t="s">
+      <c r="D55" s="12"/>
+      <c r="E55" s="28"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="B54" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="22" t="s">
+      <c r="B56" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D54" s="25" t="s">
+      <c r="D56" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E56" s="24" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="20" t="s">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="B55" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="22" t="s">
+      <c r="B57" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="24"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="17" t="s">
+      <c r="D57" s="25"/>
+      <c r="E57" s="24"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="B56" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="19" t="s">
+      <c r="B58" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D56" s="26" t="s">
+      <c r="D58" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="E56" s="24"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="17" t="s">
+      <c r="E58" s="24"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="B57" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="19" t="s">
+      <c r="B59" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="24"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E58" s="24"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="B59" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="25"/>
+      <c r="D59" s="26"/>
       <c r="E59" s="24"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B60" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60" s="25"/>
+        <v>58</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>194</v>
+      </c>
       <c r="E60" s="24"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D61" s="25"/>
       <c r="E61" s="24"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D62" s="25"/>
       <c r="E62" s="24"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B63" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D63" s="25"/>
       <c r="E63" s="24"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="17" t="s">
+      <c r="A64" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D64" s="25"/>
+      <c r="E64" s="24"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D65" s="25"/>
+      <c r="E65" s="24"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="B64" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C64" s="19" t="s">
+      <c r="B66" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="D64" s="26" t="s">
+      <c r="D66" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="E64" s="23"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
+      <c r="E66" s="23"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="B65" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="19" t="s">
+      <c r="B67" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="D65" s="26"/>
-      <c r="E65" s="23"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="9" t="s">
+      <c r="D67" s="26"/>
+      <c r="E67" s="23"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="11" t="s">
+      <c r="B68" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D66" s="12"/>
-      <c r="E66" s="12"/>
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="D64:D65"/>
+  <mergeCells count="12">
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E56:E65"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="D60:D65"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E54:E63"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D63"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E43:E46"/>
-    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E45:E48"/>
+    <mergeCell ref="E53:E55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Have basic tree rebuild
Must update funccalls for valid parse tree. More inspection on other
Basic.Elements necessary
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="222">
   <si>
     <t>→</t>
   </si>
@@ -376,9 +376,6 @@
     <t>_PARAMS1_</t>
   </si>
   <si>
-    <t>function var (_PARAMS0_) _BLOCKSTMT_</t>
-  </si>
-  <si>
     <t>_VALUE_</t>
   </si>
   <si>
@@ -689,6 +686,12 @@
   </si>
   <si>
     <t>__PRECEDENCE5__ &lt;operatorsPrecedence5&gt; _VALUEOREXPR_</t>
+  </si>
+  <si>
+    <t>function var (_PARAMS0_) _SCOPE_</t>
+  </si>
+  <si>
+    <t>_SCOPE_</t>
   </si>
 </sst>
 </file>
@@ -838,17 +841,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1758,10 +1761,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1800,7 +1803,7 @@
         <v>90</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -1817,7 +1820,7 @@
         <v>113</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>17</v>
@@ -1831,13 +1834,13 @@
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>116</v>
+        <v>220</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>112</v>
@@ -1851,13 +1854,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1868,50 +1871,45 @@
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>0</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="B7" s="13"/>
       <c r="C7" s="8" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>148</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>149</v>
+        <v>23</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
@@ -1919,19 +1917,19 @@
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>112</v>
@@ -1939,39 +1937,39 @@
     </row>
     <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
-        <v>109</v>
+        <v>80</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>149</v>
+        <v>22</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
-        <v>77</v>
+        <v>109</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>111</v>
@@ -1979,19 +1977,19 @@
     </row>
     <row r="12" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>201</v>
+        <v>92</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>148</v>
+        <v>11</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>111</v>
@@ -1999,33 +1997,36 @@
     </row>
     <row r="13" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>12</v>
+        <v>198</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>154</v>
+        <v>100</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>155</v>
+        <v>20</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>12</v>
@@ -2033,16 +2034,16 @@
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>12</v>
@@ -2050,16 +2051,16 @@
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>12</v>
@@ -2067,74 +2068,76 @@
     </row>
     <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>217</v>
+        <v>138</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>218</v>
+        <v>122</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>219</v>
+        <v>144</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>152</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="B19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F19" s="27"/>
+      <c r="F19" s="8" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F20" s="27"/>
+      <c r="E20" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>0</v>
@@ -2142,637 +2145,652 @@
       <c r="C21" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E21" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F21" s="27"/>
+      <c r="E21" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F22" s="27"/>
+        <v>211</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>197</v>
-      </c>
-      <c r="F23" s="27"/>
+      <c r="E23" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>0</v>
-      </c>
+      <c r="A24" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B24" s="13"/>
       <c r="C24" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>152</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F24" s="25"/>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B25" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
       <c r="F25" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="F26" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F27" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G27" s="8" t="s">
         <v>151</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>203</v>
+        <v>123</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>147</v>
+        <v>150</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>131</v>
-      </c>
       <c r="F29" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B31" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="8" t="s">
+      <c r="E31" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="G31" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F31" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="14" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B38" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C38" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>157</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="7" t="s">
-        <v>168</v>
+      <c r="A43" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>202</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="28" t="s">
-        <v>141</v>
+      <c r="A45" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="12"/>
+      <c r="E46" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="28"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="28"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="28"/>
     </row>
-    <row r="49" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>105</v>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="12"/>
+      <c r="E49" s="28"/>
+    </row>
+    <row r="50" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C52" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="28" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>156</v>
+        <v>33</v>
       </c>
       <c r="D54" s="12"/>
-      <c r="E54" s="28"/>
+      <c r="E54" s="28" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>0</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="28"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B56" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="E56" s="24" t="s">
-        <v>143</v>
-      </c>
+      <c r="A56" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="28"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="20" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B57" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C57" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="25"/>
-      <c r="E57" s="24"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D58" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="E58" s="24"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="26"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C59" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="E59" s="26"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D59" s="26"/>
-      <c r="E59" s="24"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B60" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="E60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="25"/>
-      <c r="E61" s="24"/>
+        <v>58</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E61" s="26"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="20" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B62" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D62" s="25"/>
-      <c r="E62" s="24"/>
+        <v>60</v>
+      </c>
+      <c r="D62" s="27"/>
+      <c r="E62" s="26"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B63" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="25"/>
-      <c r="E63" s="24"/>
+        <v>62</v>
+      </c>
+      <c r="D63" s="27"/>
+      <c r="E63" s="26"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B64" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D64" s="25"/>
-      <c r="E64" s="24"/>
+        <v>64</v>
+      </c>
+      <c r="D64" s="27"/>
+      <c r="E64" s="26"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D65" s="27"/>
+      <c r="E65" s="26"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D65" s="25"/>
-      <c r="E65" s="24"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>210</v>
-      </c>
-      <c r="E66" s="23"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="26"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D67" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="E67" s="23"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="B67" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>209</v>
-      </c>
-      <c r="D67" s="26"/>
-      <c r="E67" s="23"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="9" t="s">
+      <c r="D68" s="24"/>
+      <c r="E68" s="23"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B68" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="11" t="s">
+      <c r="B69" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="12"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E56:E65"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="D60:D65"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E46:E49"/>
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="D67:D68"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E45:E48"/>
-    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E57:E66"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D61:D66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Quite a bit of updating to CFG and Bindings
About to implement new patterning for bindings
</commit_message>
<xml_diff>
--- a/CFG.xlsx
+++ b/CFG.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="239">
   <si>
     <t>→</t>
   </si>
@@ -379,9 +379,6 @@
     <t>_VALUE_</t>
   </si>
   <si>
-    <t>_BLOCKSTMT_ _ELSEIF_</t>
-  </si>
-  <si>
     <t>_FUNCCALL_</t>
   </si>
   <si>
@@ -394,9 +391,6 @@
     <t>","</t>
   </si>
   <si>
-    <t xml:space="preserve"> = _EXPR_</t>
-  </si>
-  <si>
     <t>( _ARGS0_ )</t>
   </si>
   <si>
@@ -436,9 +430,6 @@
     <t>_VAREXPR_</t>
   </si>
   <si>
-    <t>elseif ( _EXPR_ )  _THEN_ | else _BLOCKSTMT_ | epsilon</t>
-  </si>
-  <si>
     <t>_VARDEF_ | _FUNCCALL_</t>
   </si>
   <si>
@@ -487,9 +478,6 @@
     <t>_INPUT_</t>
   </si>
   <si>
-    <t>input var</t>
-  </si>
-  <si>
     <t>input</t>
   </si>
   <si>
@@ -688,17 +676,234 @@
     <t>__PRECEDENCE5__ &lt;operatorsPrecedence5&gt; _VALUEOREXPR_</t>
   </si>
   <si>
-    <t>function var (_PARAMS0_) _SCOPE_</t>
-  </si>
-  <si>
     <t>_SCOPE_</t>
+  </si>
+  <si>
+    <t>SCOPE</t>
+  </si>
+  <si>
+    <t>VAROUT</t>
+  </si>
+  <si>
+    <t>CALCULATION</t>
+  </si>
+  <si>
+    <t>FUNCCALL</t>
+  </si>
+  <si>
+    <t>LITERAL</t>
+  </si>
+  <si>
+    <t>PARAM</t>
+  </si>
+  <si>
+    <t>STOP</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">function </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>var</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_PARAMS0_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_SCOPE_</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if ( </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_EXPR_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_SCOPE_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_ELSEIF_</t>
+    </r>
+  </si>
+  <si>
+    <t>FUNCDEF (VAROUT, PARAM, SCOPE)</t>
+  </si>
+  <si>
+    <t>OUTPUT (CALCULATION)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">echo </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_EXPR_</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>input</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> var</t>
+    </r>
+  </si>
+  <si>
+    <t>INPUT (VAROUT)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>_EXPR_</t>
+    </r>
+  </si>
+  <si>
+    <t>VARDEF (CALCULATION)</t>
+  </si>
+  <si>
+    <t>Special Bindings</t>
+  </si>
+  <si>
+    <t>IF &lt;-- ELSE</t>
+  </si>
+  <si>
+    <t>VAROUT &lt;-- FUNCCALL</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>else _ELSEIF_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> | epsilon</t>
+    </r>
+  </si>
+  <si>
+    <t>if (_EXPR_) _SCOPE_ _ELSE_ | _SCOPE_</t>
+  </si>
+  <si>
+    <t>Optimized Element Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,8 +932,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,6 +997,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -784,7 +1022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -841,11 +1079,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -853,9 +1094,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1761,17 +2017,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G69"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="59.6640625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" customWidth="1"/>
     <col min="5" max="5" width="38" customWidth="1"/>
     <col min="6" max="6" width="39.6640625" customWidth="1"/>
     <col min="7" max="7" width="35.109375" style="3" customWidth="1"/>
@@ -1785,6 +2041,9 @@
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1803,7 +2062,7 @@
         <v>90</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>7</v>
@@ -1820,7 +2079,7 @@
         <v>113</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>17</v>
@@ -1834,13 +2093,16 @@
         <v>0</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>220</v>
+        <v>224</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>226</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>112</v>
@@ -1854,13 +2116,16 @@
         <v>0</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>222</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1871,28 +2136,31 @@
         <v>0</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>221</v>
+      <c r="A7" s="29" t="s">
+        <v>216</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="8" t="s">
         <v>109</v>
       </c>
+      <c r="D7" s="8" t="s">
+        <v>217</v>
+      </c>
       <c r="E7" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1903,56 +2171,45 @@
         <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>93</v>
+        <v>225</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>23</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
-        <v>79</v>
+      <c r="A9" s="29" t="s">
+        <v>81</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>117</v>
+        <v>236</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>148</v>
+        <v>22</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:7" s="32" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>112</v>
+      <c r="B10" s="31"/>
+      <c r="C10" s="32" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -1966,10 +2223,10 @@
         <v>97</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>111</v>
@@ -1989,7 +2246,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>111</v>
@@ -2003,13 +2260,13 @@
         <v>0</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>111</v>
@@ -2023,7 +2280,10 @@
         <v>0</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>100</v>
+        <v>228</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>227</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>20</v>
@@ -2034,16 +2294,19 @@
     </row>
     <row r="15" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>153</v>
+        <v>229</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>230</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>12</v>
@@ -2051,16 +2314,16 @@
     </row>
     <row r="16" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>12</v>
@@ -2068,16 +2331,19 @@
     </row>
     <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>122</v>
+        <v>231</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>232</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>12</v>
@@ -2085,22 +2351,22 @@
     </row>
     <row r="18" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2111,87 +2377,90 @@
         <v>0</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>188</v>
+        <v>184</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="F20" s="25"/>
+        <v>186</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="24"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B21" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="F21" s="25"/>
+        <v>208</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="F22" s="25"/>
+        <v>207</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B23" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="F23" s="25"/>
+        <v>211</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F23" s="24"/>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B24" s="13"/>
       <c r="C24" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="E24" s="25" t="s">
-        <v>196</v>
-      </c>
-      <c r="F24" s="25"/>
+        <v>215</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F24" s="24"/>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
@@ -2201,110 +2470,113 @@
         <v>0</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B26" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B27" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C27" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="8" t="s">
-        <v>127</v>
-      </c>
       <c r="F27" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.3">
@@ -2318,479 +2590,532 @@
         <v>8</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F32" s="8"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C33" s="8"/>
+      <c r="D33" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" t="s">
+        <v>235</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
+      <c r="D37" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+      <c r="B42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14" t="s">
+      <c r="B43" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="B37" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14" t="s">
+      <c r="B44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="B38" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="8" t="s">
+      <c r="B45" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E50" s="25"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E51" s="25"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E52" s="25"/>
+    </row>
+    <row r="53" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" s="34"/>
+      <c r="B55" s="35"/>
+      <c r="C55" s="36"/>
+      <c r="D55" s="33" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D57" s="12"/>
+      <c r="E57" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="D58" s="12"/>
+      <c r="E58" s="25"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="E59" s="25"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D60" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="E60" s="27" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="28"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C48" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="28"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="28"/>
-    </row>
-    <row r="50" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="B50" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C55" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="28"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C56" s="11" t="s">
-        <v>187</v>
-      </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="28"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="B57" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="E57" s="26" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C58" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="D58" s="27"/>
-      <c r="E58" s="26"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C59" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="D59" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="E59" s="26"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C60" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D60" s="24"/>
-      <c r="E60" s="26"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B61" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="D61" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E61" s="26"/>
+        <v>56</v>
+      </c>
+      <c r="D61" s="28"/>
+      <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="B62" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C62" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="27"/>
-      <c r="E62" s="26"/>
+      <c r="A62" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" s="26" t="s">
+        <v>188</v>
+      </c>
+      <c r="E62" s="27"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C63" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="27"/>
-      <c r="E63" s="26"/>
+      <c r="A63" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="26"/>
+      <c r="E63" s="27"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="20" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B64" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D64" s="27"/>
-      <c r="E64" s="26"/>
+        <v>58</v>
+      </c>
+      <c r="D64" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="E64" s="27"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="20" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B65" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D65" s="27"/>
-      <c r="E65" s="26"/>
+        <v>60</v>
+      </c>
+      <c r="D65" s="28"/>
+      <c r="E65" s="27"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="20" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B66" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C66" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D66" s="28"/>
+      <c r="E66" s="27"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D67" s="28"/>
+      <c r="E67" s="27"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C68" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" s="28"/>
+      <c r="E68" s="27"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="27"/>
-      <c r="E66" s="26"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A67" s="17" t="s">
+      <c r="D69" s="28"/>
+      <c r="E69" s="27"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="D70" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="B67" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C67" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="D67" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="E67" s="23"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C68" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="D68" s="24"/>
-      <c r="E68" s="23"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="9" t="s">
+      <c r="E70" s="23"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D71" s="26"/>
+      <c r="E71" s="23"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B69" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="11" t="s">
+      <c r="B72" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="D69" s="12"/>
-      <c r="E69" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E60:E69"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="D64:D69"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E46:E49"/>
-    <mergeCell ref="E54:E56"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E57:E66"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="D61:D66"/>
+    <mergeCell ref="E49:E52"/>
+    <mergeCell ref="E57:E59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>